<commit_message>
Ajout explication pour tâche GP05
</commit_message>
<xml_diff>
--- a/Documentation/Note d'équipe/Planification sprints.xlsx
+++ b/Documentation/Note d'équipe/Planification sprints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Session_8\6DY\GrandProphete\GrandsProphetes\Documentation\Note d'équipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ÉCOLE SESSION 6\Projet fin\GrandsProphetes\Documentation\Note d'équipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D7593A-F0AC-4425-8B6C-C30636C94338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910E2B78-0961-4A48-B522-24F6A8E1F63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A238F9CB-7619-4BEE-9043-D0C8AF98FF35}"/>
+    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{A238F9CB-7619-4BEE-9043-D0C8AF98FF35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>GP18</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>Maxime &amp; Laurent</t>
+  </si>
+  <si>
+    <t>Cette tâche a été 3h plus long que prévu, car la libray utiliser est très limité
+ dans son choix d'option d'affichage alors j'ai du trouver un solution alternative
+Problème: Faire afficher une image et pouvoir déclencher une action lorsque le curseur passe dessus.
+Solution: Mettre l'image dans un button retirer le background de l'image.</t>
   </si>
 </sst>
 </file>
@@ -164,19 +170,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -196,7 +205,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -495,412 +504,429 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:I16"/>
+      <selection activeCell="G8" sqref="G8:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" customWidth="1"/>
-    <col min="6" max="6" width="25.21875" customWidth="1"/>
+    <col min="1" max="1" width="9.3046875" customWidth="1"/>
+    <col min="3" max="3" width="11.23046875" customWidth="1"/>
+    <col min="6" max="6" width="25.23046875" customWidth="1"/>
+    <col min="9" max="9" width="101.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="2"/>
       <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>5</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
       <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>10</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
       <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>12</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
       <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
       <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>12</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="F7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>24</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
       <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>3</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>6</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="F10" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
       <c r="F11" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
       <c r="F12" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" ht="78.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>6</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2"/>
       <c r="F13" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>6</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
       <c r="F14" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>8</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
       <c r="F15" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>5</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
       <c r="F16" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>8</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
       <c r="F17" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <f>SUM(B3:C24)</f>
         <v>119</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="G17:I17"/>
@@ -917,41 +943,29 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout explication tache GP08, GP13, GP14, GP18
</commit_message>
<xml_diff>
--- a/Documentation/Note d'équipe/Planification sprints.xlsx
+++ b/Documentation/Note d'équipe/Planification sprints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ÉCOLE SESSION 6\Projet fin\GrandsProphetes\Documentation\Note d'équipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Session_8\6DY\GrandProphete\GrandsProphetes\Documentation\Note d'équipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910E2B78-0961-4A48-B522-24F6A8E1F63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BA1658-7EDB-4E51-902F-E4E079CDE5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{A238F9CB-7619-4BEE-9043-D0C8AF98FF35}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A238F9CB-7619-4BEE-9043-D0C8AF98FF35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>GP18</t>
   </si>
@@ -135,6 +135,19 @@
  dans son choix d'option d'affichage alors j'ai du trouver un solution alternative
 Problème: Faire afficher une image et pouvoir déclencher une action lorsque le curseur passe dessus.
 Solution: Mettre l'image dans un button retirer le background de l'image.</t>
+  </si>
+  <si>
+    <t>Un gros bug a demandé un nombre important de ressources afin de le corriger. Il s'agit d'un bug qui apparaissait rarement (environ 1 fois sur 10) et qui était causé par plus d'une erreur de codage. Samuel a été le principal programmeur a chercher la solution, mais a aussi été aidé par Laurent, Maxime et Justin
+Il va être nécessaire d'accorder encore quelques heures au prochain sprint pour cette tache afin de terminer le merge de la tache GP05/GP06 ainsi que celui du main contenant tout les commentaires/documentations qui risque de causer quelques conflits.</t>
+  </si>
+  <si>
+    <t>Justin &amp; Samuel</t>
+  </si>
+  <si>
+    <t>Cette tache n'étant pas aussi primordial que GP08, elle n'a pas été fait autant que voulu durant le sprint suite au problème de GP08. Elle sera transféré au prochain sprint</t>
+  </si>
+  <si>
+    <t>---</t>
   </si>
 </sst>
 </file>
@@ -170,10 +183,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,10 +198,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -205,7 +221,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -503,414 +519,453 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5432DBD3-68DC-4F34-8D1E-879A62928BB7}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:I8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.3046875" customWidth="1"/>
-    <col min="3" max="3" width="11.23046875" customWidth="1"/>
-    <col min="6" max="6" width="25.23046875" customWidth="1"/>
-    <col min="9" max="9" width="101.84375" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="6" max="6" width="25.21875" customWidth="1"/>
+    <col min="9" max="9" width="101.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="3"/>
       <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>5</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="E3" s="3"/>
       <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>10</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>12</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3"/>
       <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>12</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3"/>
       <c r="F7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>24</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>3</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
       <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>6</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
       <c r="F10" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <v>2</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <v>10</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
       <c r="F12" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="78.45" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" ht="78.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <v>6</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3">
         <v>9</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="3"/>
       <c r="F13" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3"/>
       <c r="F14" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>8</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
       <c r="F15" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="3">
         <v>5</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
       <c r="F16" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="3">
         <v>8</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
       <c r="F17" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="3">
         <f>SUM(B3:C24)</f>
         <v>119</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3">
+        <f>SUM(D3:E24)</f>
+        <v>42.5</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="G10:I10"/>
@@ -927,45 +982,25 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modification chemin critique et Planification sprints
</commit_message>
<xml_diff>
--- a/Documentation/Note d'équipe/Planification sprints.xlsx
+++ b/Documentation/Note d'équipe/Planification sprints.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\battl\Desktop\ProjetFinTech\GrandsProphetes\Documentation\Note d'équipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Session_8\6DY\GrandProphete\GrandsProphetes\Documentation\Note d'équipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336381E5-B5C2-498D-AADB-75C7AD0DEEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F262D83-9DFD-4804-86FA-F285E8DCFD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A238F9CB-7619-4BEE-9043-D0C8AF98FF35}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A238F9CB-7619-4BEE-9043-D0C8AF98FF35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="55">
   <si>
     <t>GP18</t>
   </si>
@@ -172,6 +173,42 @@
   </si>
   <si>
     <t>Justin</t>
+  </si>
+  <si>
+    <t>GP37</t>
+  </si>
+  <si>
+    <t>GP34</t>
+  </si>
+  <si>
+    <t>GP28</t>
+  </si>
+  <si>
+    <t>GP07</t>
+  </si>
+  <si>
+    <t>GP35</t>
+  </si>
+  <si>
+    <t>Maxime</t>
+  </si>
+  <si>
+    <t>Samuel, Kevin, Raphaël</t>
+  </si>
+  <si>
+    <t>Samuel, Laurent</t>
+  </si>
+  <si>
+    <t>Justin, Maxime</t>
+  </si>
+  <si>
+    <t>GP22-1</t>
+  </si>
+  <si>
+    <t>GP22-2</t>
+  </si>
+  <si>
+    <t>Planification Sprints</t>
   </si>
 </sst>
 </file>
@@ -213,10 +250,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -225,7 +262,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -245,7 +282,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -543,11 +580,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5432DBD3-68DC-4F34-8D1E-879A62928BB7}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:I9"/>
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.21875" customWidth="1"/>
@@ -556,51 +593,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="2"/>
       <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>5</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
         <v>18</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="2"/>
       <c r="F3" t="s">
         <v>34</v>
       </c>
@@ -614,14 +651,14 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>10</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
         <v>10</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="2"/>
       <c r="F4" t="s">
         <v>19</v>
       </c>
@@ -635,56 +672,56 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>12</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
         <v>12</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="2"/>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
         <v>2</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="2"/>
       <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>12</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
         <v>2</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="2"/>
       <c r="F7" t="s">
         <v>18</v>
       </c>
@@ -698,14 +735,14 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>24</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
         <v>12</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="2"/>
       <c r="F8" t="s">
         <v>26</v>
       </c>
@@ -719,35 +756,35 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>3</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="2"/>
       <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>6</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="2"/>
       <c r="F10" t="s">
         <v>23</v>
       </c>
@@ -761,259 +798,271 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
         <v>2</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="2"/>
       <c r="F11" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
         <v>8.5</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="2"/>
       <c r="F12" t="s">
         <v>24</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="78.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>6</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
         <v>9</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="2"/>
       <c r="F13" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>6</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
         <v>6</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="2"/>
       <c r="F14" t="s">
         <v>20</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>8</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
         <v>8.25</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="2"/>
       <c r="F15" t="s">
         <v>24</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>5</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2">
         <v>5</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="2"/>
       <c r="F16" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>8</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2">
         <v>3</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="2"/>
       <c r="F17" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <f>SUM(B3:C24)</f>
         <v>119</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2">
         <f>SUM(D3:E24)</f>
         <v>97.75</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="E25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="G17:I17"/>
@@ -1030,41 +1079,489 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F37B18-6DC2-4F92-80AB-8018DE843EF7}">
+  <dimension ref="A1:I26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="87.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="2">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="2">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="2">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="2">
+        <f>SUM(B3:C25)</f>
+        <v>63</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2">
+        <f>SUM(D3:E25)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="76">
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="G9:I9"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G5:I5"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout des tache dans la Planification sprints
</commit_message>
<xml_diff>
--- a/Documentation/Note d'équipe/Planification sprints.xlsx
+++ b/Documentation/Note d'équipe/Planification sprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Session_8\6DY\GrandProphete\GrandsProphetes\Documentation\Note d'équipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C6EED4-0576-4653-A355-A49EA0070274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E0624A-FFEA-477E-8B3B-15993E195FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A238F9CB-7619-4BEE-9043-D0C8AF98FF35}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>GP18</t>
   </si>
@@ -212,6 +212,15 @@
   </si>
   <si>
     <t>Le temps a bien été estimé. Il a pris en compte les possibilités de problèmes reliés au merge (qui ont eu lieu, mais de moins grandes ampleurs que celui du sprint précédent). La tache maintenant terminer, nous pouvons par la suite procéder au développement des dernières fonctionnalités, aux tests des méthodes et à la rédaction des documentations.</t>
+  </si>
+  <si>
+    <t>GP38</t>
+  </si>
+  <si>
+    <t>GP39</t>
+  </si>
+  <si>
+    <t>Samuel, Kevin</t>
   </si>
 </sst>
 </file>
@@ -253,10 +262,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -265,7 +274,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,51 +605,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="2"/>
       <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>5</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
         <v>18</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="2"/>
       <c r="F3" t="s">
         <v>34</v>
       </c>
@@ -654,14 +663,14 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>10</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
         <v>10</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="2"/>
       <c r="F4" t="s">
         <v>19</v>
       </c>
@@ -675,56 +684,56 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>12</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
         <v>12</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="2"/>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
         <v>2</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="2"/>
       <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>12</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
         <v>2</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="2"/>
       <c r="F7" t="s">
         <v>18</v>
       </c>
@@ -738,14 +747,14 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>24</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
         <v>12</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="2"/>
       <c r="F8" t="s">
         <v>26</v>
       </c>
@@ -759,35 +768,35 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>3</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="2"/>
       <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>6</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="2"/>
       <c r="F10" t="s">
         <v>23</v>
       </c>
@@ -801,259 +810,271 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
         <v>2</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="2"/>
       <c r="F11" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
         <v>8.5</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="2"/>
       <c r="F12" t="s">
         <v>24</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="78.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>6</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
         <v>9</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="2"/>
       <c r="F13" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>6</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
         <v>6</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="2"/>
       <c r="F14" t="s">
         <v>20</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>8</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
         <v>8.25</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="2"/>
       <c r="F15" t="s">
         <v>24</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>5</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2">
         <v>5</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="2"/>
       <c r="F16" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>8</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2">
         <v>3</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="2"/>
       <c r="F17" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <f>SUM(B3:C24)</f>
         <v>119</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2">
         <f>SUM(D3:E24)</f>
         <v>97.75</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="E25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="G17:I17"/>
@@ -1070,41 +1091,29 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1115,7 +1124,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:I7"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1126,49 +1135,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="2"/>
       <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
       <c r="F3" t="s">
         <v>24</v>
       </c>
@@ -1180,12 +1189,12 @@
       <c r="A4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
       <c r="F4" t="s">
         <v>22</v>
       </c>
@@ -1197,31 +1206,31 @@
       <c r="A5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
       <c r="F5" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>6</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
         <v>6</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="2"/>
       <c r="F6" t="s">
         <v>18</v>
       </c>
@@ -1235,12 +1244,12 @@
       <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="F7" t="s">
         <v>48</v>
       </c>
@@ -1252,12 +1261,12 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>3</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
       <c r="F8" t="s">
         <v>48</v>
       </c>
@@ -1269,29 +1278,29 @@
       <c r="A9" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>6</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>10</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="F10" t="s">
         <v>22</v>
       </c>
@@ -1303,222 +1312,255 @@
       <c r="A11" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>8</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
       <c r="F11" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>7</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
       <c r="F12" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>6</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
       <c r="F13" t="s">
         <v>50</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>5</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
       <c r="F14" t="s">
         <v>42</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>3</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
       <c r="F15" t="s">
         <v>23</v>
       </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <f>SUM(B3:C25)</f>
-        <v>63</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3">
+        <v>68</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2">
         <f>SUM(D3:E25)</f>
         <v>6</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="E26" s="2"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="G14:I14"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="G10:I10"/>
@@ -1528,48 +1570,31 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>